<commit_message>
Update DM integration test fixture
</commit_message>
<xml_diff>
--- a/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/domain-members-and-hierarchies-DOME-2018-1.xlsx
+++ b/yti-taxgen-test-commons/src/main/resources/test_fixtures/rds_source_config/dm_integration_fixture/domain-members-and-hierarchies-DOME-2018-1.xlsx
@@ -6,7 +6,8 @@
     <sheet sheetId="1" name="CodeSchemes" r:id="rId4"/>
     <sheet sheetId="2" name="Codes" r:id="rId5"/>
     <sheet sheetId="3" name="Extensions" r:id="rId6"/>
-    <sheet sheetId="4" name="Members_HIER" r:id="rId7"/>
+    <sheet sheetId="4" name="Members_EDA-H1" r:id="rId7"/>
+    <sheet sheetId="5" name="Members_HIER" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -17,11 +18,41 @@
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,10 +83,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="2" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="3" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="4" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" numFmtId="0" fontId="5" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -76,89 +112,89 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="34.1"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="17.6"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="15.400000000000002"/>
-    <col min="5" max="5" bestFit="1" customWidth="1" width="9.9"/>
-    <col min="6" max="6" bestFit="1" customWidth="1" width="13.200000000000001"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="33.0"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="26.4"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="23.099999999999998"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="14.85"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
     <col min="7" max="7" bestFit="1" customWidth="1" width="23.1"/>
-    <col min="8" max="8" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="9" max="9" bestFit="1" customWidth="1" width="14.3"/>
-    <col min="10" max="10" bestFit="1" customWidth="1" width="16.5"/>
-    <col min="11" max="11" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="12" max="12" bestFit="1" customWidth="1" width="11.0"/>
-    <col min="13" max="13" bestFit="1" customWidth="1" width="14.3"/>
-    <col min="14" max="14" bestFit="1" customWidth="1" width="18.700000000000003"/>
+    <col min="8" max="8" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="9" max="9" bestFit="1" customWidth="1" width="21.45"/>
+    <col min="10" max="10" bestFit="1" customWidth="1" width="24.75"/>
+    <col min="11" max="11" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="12" max="12" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="13" max="13" bestFit="1" customWidth="1" width="21.45"/>
+    <col min="14" max="14" bestFit="1" customWidth="1" width="28.049999999999997"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>CODEVALUE</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>INFORMATIONDOMAIN</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>LANGUAGECODE</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>DEFAULTCODE</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>PREFLABEL_FI</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>PREFLABEL_EN</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>DESCRIPTION_FI</t>
         </is>
       </c>
-      <c r="J1" s="0" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>DESCRIPTION_EN</t>
         </is>
       </c>
-      <c r="K1" s="0" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>STARTDATE</t>
         </is>
       </c>
-      <c r="L1" s="0" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>ENDDATE</t>
         </is>
       </c>
-      <c r="M1" s="0" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>CODESSHEET</t>
         </is>
       </c>
-      <c r="N1" s="0" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>EXTENSIONSSHEET</t>
         </is>
@@ -167,7 +203,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>5cb2e7e8-5b85-4bf0-b94e-c289974348fe</t>
+          <t>142e10e1-4e52-43f6-99e8-a21a5f8ec354</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -226,71 +262,71 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="12.100000000000001"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="11.0"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="9.9"/>
-    <col min="5" max="5" bestFit="1" customWidth="1" width="14.3"/>
-    <col min="6" max="6" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="7" max="7" bestFit="1" customWidth="1" width="17.6"/>
-    <col min="8" max="8" bestFit="1" customWidth="1" width="16.5"/>
-    <col min="9" max="9" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="10" max="10" bestFit="1" customWidth="1" width="11.0"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="35.2"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="14.85"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="29.700000000000003"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="7" max="7" bestFit="1" customWidth="1" width="21.45"/>
+    <col min="8" max="8" bestFit="1" customWidth="1" width="24.75"/>
+    <col min="9" max="9" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="10" max="10" bestFit="1" customWidth="1" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>CODEVALUE</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>BROADER</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>PREFLABEL_FI</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>PREFLABEL_EN</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>DESCRIPTION_FI</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>DESCRIPTION_EN</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>STARTDATE</t>
         </is>
       </c>
-      <c r="J1" s="0" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>ENDDATE</t>
         </is>
@@ -299,12 +335,12 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>263ff260-543a-4add-95b4-16c743211c56</t>
+          <t>4e8015ad-fcc7-47d8-822d-0f924a591cda</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>EDA-x1</t>
         </is>
       </c>
       <c r="C2" s="0"/>
@@ -315,22 +351,58 @@
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Member (fi, label)</t>
+          <t>DOME member duplicating EDA code</t>
         </is>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>Member (fi, description)</t>
+          <t/>
         </is>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0" t="inlineStr">
         <is>
+          <t>2018-12-31</t>
+        </is>
+      </c>
+      <c r="J2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>227bbfbf-d2da-449b-8776-302b82925039</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>DRAFT</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Member (fi, label)</t>
+        </is>
+      </c>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>Member (fi, description)</t>
+        </is>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
           <t>2018-10-31</t>
         </is>
       </c>
-      <c r="J2" s="0"/>
+      <c r="J3" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
@@ -346,65 +418,65 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="12.100000000000001"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="9.9"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="16.5"/>
-    <col min="5" max="5" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="6" max="6" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="7" max="7" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="8" max="8" bestFit="1" customWidth="1" width="11.0"/>
-    <col min="9" max="9" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="18.15"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="24.75"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="28.6"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="7" max="7" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="8" max="8" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="9" max="9" bestFit="1" customWidth="1" width="24.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>CODEVALUE</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>STATUS</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>PROPERTYTYPE</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>PREFLABEL_FI</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>PREFLABEL_EN</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>STARTDATE</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>ENDDATE</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>MEMBERSSHEET</t>
         </is>
@@ -413,12 +485,12 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>54fce058-b41e-40d1-b714-daf97821daf1</t>
+          <t>547ae846-b7c4-4b8d-a165-a3cf807e9db1</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>HIER</t>
+          <t>EDA-H1</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -433,17 +505,56 @@
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Hierarchy (fi, label)</t>
+          <t>DOME hierarchy duplicating EDA code</t>
         </is>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>2018-10-31</t>
+          <t>2018-12-31</t>
         </is>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>Members_EDA-H1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>dc0a8827-8f95-4eec-9057-4d44f00976fc</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>HIER</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>DRAFT</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>definitionHierarchy</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Hierarchy (fi, label)</t>
+        </is>
+      </c>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>2018-10-31</t>
+        </is>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0" t="inlineStr">
         <is>
           <t>Members_HIER</t>
         </is>
@@ -463,53 +574,119 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="6.6"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="11.549999999999999"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="7" max="7" bestFit="1" customWidth="1" width="16.5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>CODE</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>RELATION</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>PREFLABEL_FI</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>PREFLABEL_EN</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>STARTDATE</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>ENDDATE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <printOptions verticalCentered="0" horizontalCentered="0" headings="0" gridLines="0"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="1" customWidth="1" width="31.900000000000002"/>
-    <col min="2" max="2" bestFit="1" customWidth="1" width="7.700000000000001"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="9.9"/>
-    <col min="4" max="4" bestFit="1" customWidth="1" width="14.3"/>
-    <col min="5" max="5" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="6" max="6" bestFit="1" customWidth="1" width="13.200000000000001"/>
-    <col min="7" max="7" bestFit="1" customWidth="1" width="11.0"/>
+    <col min="1" max="1" bestFit="1" customWidth="1" width="30.800000000000004"/>
+    <col min="2" max="2" bestFit="1" customWidth="1" width="11.549999999999999"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="14.85"/>
+    <col min="4" max="4" bestFit="1" customWidth="1" width="16.5"/>
+    <col min="5" max="5" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="6" max="6" bestFit="1" customWidth="1" width="19.799999999999997"/>
+    <col min="7" max="7" bestFit="1" customWidth="1" width="16.5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>CODE</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>RELATION</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>PREFLABEL_FI</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>PREFLABEL_EN</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>STARTDATE</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" s="7" t="inlineStr">
         <is>
           <t>ENDDATE</t>
         </is>
@@ -518,7 +695,7 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>d92580a0-579b-4f80-803c-9ee17ee2ac6a</t>
+          <t>45395986-ece0-4f2c-847f-3af8bbd0ba6b</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">

</xml_diff>